<commit_message>
Multiple students per project; supervisor preferences; CSV removed; I/O performance tweaks
</commit_message>
<xml_diff>
--- a/pdn_project_allocation/testdata/test6_excel.xlsx
+++ b/pdn_project_allocation/testdata/test6_excel.xlsx
@@ -8,7 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="test4_n10_multiple_ties" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Projects" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Student_preferences" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Supervisor_preferences" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,42 +22,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Project_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max_number_of_students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P11</t>
+  </si>
   <si>
     <t xml:space="preserve">N=10 with multiple ties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P11</t>
   </si>
   <si>
     <t xml:space="preserve">S1</t>
@@ -100,6 +108,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,10 +190,133 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -197,45 +329,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -249,7 +381,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -263,7 +395,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -277,7 +409,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -291,7 +423,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>1</v>
@@ -305,7 +437,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>1</v>
@@ -319,7 +451,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
@@ -333,7 +465,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>3</v>
@@ -347,7 +479,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>1</v>
@@ -361,7 +493,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>1</v>
@@ -382,4 +514,122 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>